<commit_message>
Clang(Dhrystone) with aggressive code promotion
</commit_message>
<xml_diff>
--- a/clang.xlsx
+++ b/clang.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="dhrystone" sheetId="2" r:id="rId1"/>
-    <sheet name="Methodology" sheetId="6" r:id="rId2"/>
+    <sheet name="code_promo" sheetId="7" r:id="rId2"/>
+    <sheet name="Methodology" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>CPU_CLK_UNHALTED.THREAD_P</t>
   </si>
@@ -85,13 +86,67 @@
   </si>
   <si>
     <t>dd_usr</t>
+  </si>
+  <si>
+    <t>BR_MISP_RETIRED.ALL_BRANCHES</t>
+  </si>
+  <si>
+    <t>ITLB_MISSES.MISS_CAUSES_A_WALK</t>
+  </si>
+  <si>
+    <t>0(0)</t>
+  </si>
+  <si>
+    <t>2(1)</t>
+  </si>
+  <si>
+    <t>3(2)</t>
+  </si>
+  <si>
+    <t>4(3)</t>
+  </si>
+  <si>
+    <t>6(4)</t>
+  </si>
+  <si>
+    <t>8(5)</t>
+  </si>
+  <si>
+    <t>10(6)</t>
+  </si>
+  <si>
+    <t>11(7)</t>
+  </si>
+  <si>
+    <t>12(10)</t>
+  </si>
+  <si>
+    <t>15(13)</t>
+  </si>
+  <si>
+    <t>17(14)</t>
+  </si>
+  <si>
+    <t>18(15)</t>
+  </si>
+  <si>
+    <t>25(16)</t>
+  </si>
+  <si>
+    <t>25(dd)</t>
+  </si>
+  <si>
+    <t>Per-execution</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,6 +185,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,12 +216,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1246,9 +1308,474 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.5" style="1" customWidth="1"/>
+    <col min="2" max="14" width="18.83203125" style="1"/>
+    <col min="15" max="15" width="18.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="18.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1412890215513.5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1394586125758</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1389793823976.5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1357437220494</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1372866476656</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1357199490610.5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1340026656613</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1334703015642.5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1331244987517</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1329376856252</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1328284266384.5</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1328910774695</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1322318274872.5</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1331954984895.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6578029997.5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6590001001.5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6623840872.5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7575524880.5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6630834432</v>
+      </c>
+      <c r="G4" s="1">
+        <v>6834442395.5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>7545425827</v>
+      </c>
+      <c r="I4" s="1">
+        <v>7556351649</v>
+      </c>
+      <c r="J4" s="1">
+        <v>7585481748.5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>7578983393</v>
+      </c>
+      <c r="L4" s="1">
+        <v>7583826062</v>
+      </c>
+      <c r="M4" s="1">
+        <v>7567049352.5</v>
+      </c>
+      <c r="N4" s="1">
+        <v>7577520840</v>
+      </c>
+      <c r="O4" s="1">
+        <v>6592402252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>469617916</v>
+      </c>
+      <c r="C5" s="1">
+        <v>342134538.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>317113708</v>
+      </c>
+      <c r="E5" s="1">
+        <v>230760732.5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>210266644.5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>166958770</v>
+      </c>
+      <c r="H5" s="1">
+        <v>106746348.5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>80982574</v>
+      </c>
+      <c r="J5" s="1">
+        <v>69688235.5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>52394159.5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>38985171.5</v>
+      </c>
+      <c r="M5" s="1">
+        <v>32235469.5</v>
+      </c>
+      <c r="N5" s="1">
+        <v>24313638.5</v>
+      </c>
+      <c r="O5" s="1">
+        <v>23981048</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>350700489</v>
+      </c>
+      <c r="C6" s="1">
+        <v>252292387</v>
+      </c>
+      <c r="D6" s="1">
+        <v>231564291</v>
+      </c>
+      <c r="E6" s="1">
+        <v>156326115</v>
+      </c>
+      <c r="F6" s="1">
+        <v>151376560.5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>116435926.5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>68555934.5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>49526771</v>
+      </c>
+      <c r="J6" s="1">
+        <v>41184229</v>
+      </c>
+      <c r="K6" s="1">
+        <v>28163147</v>
+      </c>
+      <c r="L6" s="1">
+        <v>19783128.5</v>
+      </c>
+      <c r="M6" s="1">
+        <v>14725185</v>
+      </c>
+      <c r="N6" s="1">
+        <v>9377347</v>
+      </c>
+      <c r="O6" s="1">
+        <v>8210045</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>282578043.1027</v>
+      </c>
+      <c r="C9" s="1">
+        <v>278917225.1516</v>
+      </c>
+      <c r="D9" s="1">
+        <v>277958764.79530001</v>
+      </c>
+      <c r="E9" s="1">
+        <v>271487444.0988</v>
+      </c>
+      <c r="F9" s="1">
+        <v>274573295.3312</v>
+      </c>
+      <c r="G9" s="1">
+        <v>271439898.1221</v>
+      </c>
+      <c r="H9" s="1">
+        <v>268005331.32260001</v>
+      </c>
+      <c r="I9" s="1">
+        <v>266940603.12850001</v>
+      </c>
+      <c r="J9" s="1">
+        <v>266248997.5034</v>
+      </c>
+      <c r="K9" s="1">
+        <v>265875371.25040001</v>
+      </c>
+      <c r="L9" s="1">
+        <v>265656853.27689999</v>
+      </c>
+      <c r="M9" s="1">
+        <v>265782154.93900001</v>
+      </c>
+      <c r="N9" s="1">
+        <v>264463654.9745</v>
+      </c>
+      <c r="O9" s="1">
+        <v>266390996.97909999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1315605.9994999999</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1318000.2002999999</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1324768.1745</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1515104.9761000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1326166.8864</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1366888.4791000001</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1509085.1654000001</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1511270.3297999999</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1517096.3496999999</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1515796.6786</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1516765.2124000001</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1513409.8705</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1515504.1680000001</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1318480.4504</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>93923.583199999994</v>
+      </c>
+      <c r="C11" s="1">
+        <v>68426.907699999996</v>
+      </c>
+      <c r="D11" s="1">
+        <v>63422.741600000001</v>
+      </c>
+      <c r="E11" s="1">
+        <v>46152.146500000003</v>
+      </c>
+      <c r="F11" s="1">
+        <v>42053.3289</v>
+      </c>
+      <c r="G11" s="1">
+        <v>33391.754000000001</v>
+      </c>
+      <c r="H11" s="1">
+        <v>21349.269700000001</v>
+      </c>
+      <c r="I11" s="1">
+        <v>16196.514800000001</v>
+      </c>
+      <c r="J11" s="1">
+        <v>13937.6471</v>
+      </c>
+      <c r="K11" s="1">
+        <v>10478.831899999999</v>
+      </c>
+      <c r="L11" s="1">
+        <v>7797.0343000000003</v>
+      </c>
+      <c r="M11" s="1">
+        <v>6447.0938999999998</v>
+      </c>
+      <c r="N11" s="1">
+        <v>4862.7277000000004</v>
+      </c>
+      <c r="O11" s="1">
+        <v>4796.2096000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>70140.097800000003</v>
+      </c>
+      <c r="C12" s="1">
+        <v>50458.477400000003</v>
+      </c>
+      <c r="D12" s="1">
+        <v>46312.858200000002</v>
+      </c>
+      <c r="E12" s="1">
+        <v>31265.223000000002</v>
+      </c>
+      <c r="F12" s="1">
+        <v>30275.312099999999</v>
+      </c>
+      <c r="G12" s="1">
+        <v>23287.185300000001</v>
+      </c>
+      <c r="H12" s="1">
+        <v>13711.186900000001</v>
+      </c>
+      <c r="I12" s="1">
+        <v>9905.3541999999998</v>
+      </c>
+      <c r="J12" s="1">
+        <v>8236.8457999999991</v>
+      </c>
+      <c r="K12" s="1">
+        <v>5632.6293999999998</v>
+      </c>
+      <c r="L12" s="1">
+        <v>3956.6257000000001</v>
+      </c>
+      <c r="M12" s="1">
+        <v>2945.0369999999998</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1875.4694</v>
+      </c>
+      <c r="O12" s="1">
+        <v>1642.009</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Postgres(1G, select-only) final data
</commit_message>
<xml_diff>
--- a/clang.xlsx
+++ b/clang.xlsx
@@ -293,8 +293,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -316,11 +320,15 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -599,7 +607,7 @@
   <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17:J35"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,7 +740,7 @@
         <v>1.4662309196600636</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -773,7 +781,7 @@
         <v>1.6284495019147514</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -814,7 +822,7 @@
         <v>1.2151569016298527</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -855,7 +863,7 @@
         <v>1.6312350427915381</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -896,7 +904,7 @@
         <v>1.319726043002146</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -937,7 +945,7 @@
         <v>1.021902068838302</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -978,7 +986,7 @@
         <v>1.0000027973397301</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1019,7 +1027,7 @@
         <v>1.0219021066301692</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added new results for evaluating the impact of code superpages on dtlb
</commit_message>
<xml_diff>
--- a/clang.xlsx
+++ b/clang.xlsx
@@ -1,25 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/winnie/Development/research/shared_ptp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xdong\OneDrive\Paper\git_hub\shared_ptp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_F740F62D79B1ADD581DB163033E2D3777A84950E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{57070D98-D299-42DE-90C3-819FED3CFB21}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="dhrystone" sheetId="2" r:id="rId1"/>
-    <sheet name="code_promo" sheetId="7" r:id="rId2"/>
-    <sheet name="Methodology" sheetId="6" r:id="rId3"/>
+    <sheet name="data-superpg" sheetId="8" r:id="rId1"/>
+    <sheet name="dhrystone" sheetId="2" r:id="rId2"/>
+    <sheet name="code_promo" sheetId="7" r:id="rId3"/>
+    <sheet name="Methodology" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
   <si>
     <t>CPU_CLK_UNHALTED.THREAD_P</t>
   </si>
@@ -221,16 +229,77 @@
   </si>
   <si>
     <t>M-s_L(2)/M-s_L(1)</t>
+  </si>
+  <si>
+    <t>code no superpage, data no superpage</t>
+  </si>
+  <si>
+    <t>code no superpage, data superpage</t>
+  </si>
+  <si>
+    <t>code superpage, data no superpage</t>
+  </si>
+  <si>
+    <t>code superpage, data superpage</t>
+  </si>
+  <si>
+    <t>Col C/Col B</t>
+  </si>
+  <si>
+    <t>Col D/ Col B</t>
+  </si>
+  <si>
+    <t>Col E/ Col B</t>
+  </si>
+  <si>
+    <t>DTLB_LOAD_MISSES.WALK_COMPLETED</t>
+  </si>
+  <si>
+    <t>DTLB_LOAD_MISSES.WALK_PENDING</t>
+  </si>
+  <si>
+    <t>DTLB_STORE_MISSES.WALK_COMPLETED</t>
+  </si>
+  <si>
+    <t>DTLB_STORE_MISSES.WALK_PENDING</t>
+  </si>
+  <si>
+    <t>ITLB_MISSES.WALK_PENDING</t>
+  </si>
+  <si>
+    <t>ICACHE_64B.IFTAG_STALL</t>
+  </si>
+  <si>
+    <t>CPU_CLK_UNHALTED.THREAD_P (os + usr)</t>
+  </si>
+  <si>
+    <t>INST_RETIRED.ANY_P (os + user)</t>
+  </si>
+  <si>
+    <t>INST_RETIRED.ANY_P</t>
+  </si>
+  <si>
+    <t>CYCLE_ACTIVITY.STALLS_L3_MISS</t>
+  </si>
+  <si>
+    <t>elapse time</t>
+  </si>
+  <si>
+    <t>5000 iterations</t>
+  </si>
+  <si>
+    <t>4 hyperthreads/2cores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -275,6 +344,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -293,7 +382,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -303,8 +392,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -319,8 +409,15 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="9" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
+    <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -336,6 +433,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -603,31 +703,476 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384F6F9-A13C-42B9-8587-294C53F132BC}">
+  <dimension ref="A2:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="36.8125" customWidth="1"/>
+    <col min="2" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.0625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="78.75" x14ac:dyDescent="0.5">
+      <c r="A6" s="11"/>
+      <c r="B6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="11">
+        <v>269559340.06045002</v>
+      </c>
+      <c r="C7" s="11">
+        <v>270584219.91035002</v>
+      </c>
+      <c r="D7" s="11">
+        <v>254979371.49505001</v>
+      </c>
+      <c r="E7" s="11">
+        <v>254972036.48005</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11">
+        <f>C7/B7</f>
+        <v>1.0038020565329704</v>
+      </c>
+      <c r="H7" s="11">
+        <f>D7/B7</f>
+        <v>0.94591184055380761</v>
+      </c>
+      <c r="I7" s="11">
+        <f>E7/B7</f>
+        <v>0.94588462942100715</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A8" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="11">
+        <v>47708.169950000003</v>
+      </c>
+      <c r="C8" s="11">
+        <v>47066.353499999997</v>
+      </c>
+      <c r="D8" s="11">
+        <v>3474.0246000000002</v>
+      </c>
+      <c r="E8" s="11">
+        <v>2698.9146500000002</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11">
+        <f t="shared" ref="G8:G19" si="0">C8/B8</f>
+        <v>0.98654703270587296</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" ref="H8:H19" si="1">D8/B8</f>
+        <v>7.2818232257512952E-2</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" ref="I8:I19" si="2">E8/B8</f>
+        <v>5.6571330504367835E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A9" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2674726.7326000002</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2690581.50055</v>
+      </c>
+      <c r="D9" s="11">
+        <v>193823.9283</v>
+      </c>
+      <c r="E9" s="11">
+        <v>148097.10935000001</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0059276215984083</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="1"/>
+        <v>7.2464946021454354E-2</v>
+      </c>
+      <c r="I9" s="11">
+        <f t="shared" si="2"/>
+        <v>5.5369061648417608E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="11">
+        <v>14931593.6647</v>
+      </c>
+      <c r="C10" s="11">
+        <v>15033360.7807</v>
+      </c>
+      <c r="D10" s="11">
+        <v>5605997.9632999999</v>
+      </c>
+      <c r="E10" s="11">
+        <v>5554597.0680999998</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0068155562149128</v>
+      </c>
+      <c r="H10" s="11">
+        <f t="shared" si="1"/>
+        <v>0.37544538708907021</v>
+      </c>
+      <c r="I10" s="11">
+        <f t="shared" si="2"/>
+        <v>0.37200296182929921</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A11" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="11">
+        <v>269532641.56809998</v>
+      </c>
+      <c r="C11" s="11">
+        <v>270569085.08074999</v>
+      </c>
+      <c r="D11" s="11">
+        <v>254972162.96145001</v>
+      </c>
+      <c r="E11" s="11">
+        <v>254927708.68669999</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0038453357879777</v>
+      </c>
+      <c r="H11" s="11">
+        <f t="shared" si="1"/>
+        <v>0.94597879306217125</v>
+      </c>
+      <c r="I11" s="11">
+        <f t="shared" si="2"/>
+        <v>0.94581386211172525</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11">
+        <v>19342.494200000001</v>
+      </c>
+      <c r="C12" s="11">
+        <v>19324.010600000001</v>
+      </c>
+      <c r="D12" s="11">
+        <v>3853.5345499999999</v>
+      </c>
+      <c r="E12" s="11">
+        <v>3631.0277500000002</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11">
+        <f t="shared" si="0"/>
+        <v>0.99904440452152243</v>
+      </c>
+      <c r="H12" s="11">
+        <f t="shared" si="1"/>
+        <v>0.19922635158396479</v>
+      </c>
+      <c r="I12" s="11">
+        <f t="shared" si="2"/>
+        <v>0.18772282997505046</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A13" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1585133.47765</v>
+      </c>
+      <c r="C13" s="11">
+        <v>1620427.36555</v>
+      </c>
+      <c r="D13" s="11">
+        <v>656908.25349999999</v>
+      </c>
+      <c r="E13" s="11">
+        <v>646197.75254999998</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11">
+        <f t="shared" si="0"/>
+        <v>1.022265562110469</v>
+      </c>
+      <c r="H13" s="11">
+        <f t="shared" si="1"/>
+        <v>0.41441825736586102</v>
+      </c>
+      <c r="I13" s="11">
+        <f t="shared" si="2"/>
+        <v>0.40766141253164639</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A14" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="11">
+        <v>10896.971149999999</v>
+      </c>
+      <c r="C14" s="11">
+        <v>10753.867550000001</v>
+      </c>
+      <c r="D14" s="11">
+        <v>9352.0624499999994</v>
+      </c>
+      <c r="E14" s="11">
+        <v>8825.4004999999997</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11">
+        <f t="shared" si="0"/>
+        <v>0.98686758017157838</v>
+      </c>
+      <c r="H14" s="11">
+        <f t="shared" si="1"/>
+        <v>0.85822586122933797</v>
+      </c>
+      <c r="I14" s="11">
+        <f t="shared" si="2"/>
+        <v>0.80989482109439193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="11">
+        <v>538604.22155000002</v>
+      </c>
+      <c r="C15" s="11">
+        <v>550671.14994999999</v>
+      </c>
+      <c r="D15" s="11">
+        <v>437690.78615</v>
+      </c>
+      <c r="E15" s="11">
+        <v>420984.0122</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0224040731899087</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="1"/>
+        <v>0.81263898171909899</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="2"/>
+        <v>0.78162033522219421</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="11">
+        <v>47723.016049999998</v>
+      </c>
+      <c r="C16" s="11">
+        <v>47050.125950000001</v>
+      </c>
+      <c r="D16" s="11">
+        <v>3466.6095500000001</v>
+      </c>
+      <c r="E16" s="11">
+        <v>2695.7633000000001</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11">
+        <f t="shared" si="0"/>
+        <v>0.98590009274990076</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="1"/>
+        <v>7.2640202504552318E-2</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" si="2"/>
+        <v>5.6487697616923779E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A17" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="11">
+        <v>2676890.3783499999</v>
+      </c>
+      <c r="C17" s="11">
+        <v>2692992.3051</v>
+      </c>
+      <c r="D17" s="11">
+        <v>193731.09755000001</v>
+      </c>
+      <c r="E17" s="11">
+        <v>148404.8449</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0060151610541201</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>7.2371696322287696E-2</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="2"/>
+        <v>5.5439268675422856E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A18" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="11">
+        <v>14933141.28015</v>
+      </c>
+      <c r="C18" s="11">
+        <v>15035233.9946</v>
+      </c>
+      <c r="D18" s="11">
+        <v>5608488.4069499997</v>
+      </c>
+      <c r="E18" s="11">
+        <v>5552873.8894499997</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11">
+        <f t="shared" si="0"/>
+        <v>1.006836653623957</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="1"/>
+        <v>0.37557325024475119</v>
+      </c>
+      <c r="I18" s="11">
+        <f t="shared" si="2"/>
+        <v>0.3718490159087427</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A19" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="11">
+        <v>434.24299999999999</v>
+      </c>
+      <c r="C19" s="11">
+        <v>435.87299999999999</v>
+      </c>
+      <c r="D19" s="11">
+        <v>400.45499999999998</v>
+      </c>
+      <c r="E19" s="11">
+        <v>400.55799999999999</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11">
+        <f t="shared" si="0"/>
+        <v>1.00375365866577</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="1"/>
+        <v>0.92219103128893265</v>
+      </c>
+      <c r="I19" s="11">
+        <f t="shared" si="2"/>
+        <v>0.92242822567088012</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.1875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.3125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1875" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6875" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="18.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="10.1875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -645,7 +1190,7 @@
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" s="4"/>
       <c r="B2" s="9" t="s">
         <v>61</v>
@@ -673,7 +1218,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="B3" s="1" t="s">
         <v>49</v>
       </c>
@@ -699,7 +1244,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -740,7 +1285,7 @@
         <v>1.4662309196600636</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -781,7 +1326,7 @@
         <v>1.6284495019147514</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -822,7 +1367,7 @@
         <v>1.2151569016298527</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -863,7 +1408,7 @@
         <v>1.6312350427915381</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -904,7 +1449,7 @@
         <v>1.319726043002146</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -945,7 +1490,7 @@
         <v>1.021902068838302</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -986,7 +1531,7 @@
         <v>1.0000027973397301</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1027,7 +1572,7 @@
         <v>1.0219021066301692</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1068,7 +1613,7 @@
         <v>1.1490917247568224</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>55</v>
       </c>
@@ -1117,7 +1662,7 @@
         <v>1.331621813417551</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
@@ -1166,7 +1711,7 @@
         <v>1.1075850402692589</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1215,7 +1760,7 @@
         <v>1.3330443846661637</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>58</v>
       </c>
@@ -1264,7 +1809,7 @@
         <v>1.2706539651957589</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1305,7 +1850,7 @@
         <v>1.5513870633571372</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" s="5" t="s">
         <v>30</v>
       </c>
@@ -1346,7 +1891,7 @@
         <v>1.0000685044499933</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1387,7 +1932,7 @@
         <v>1.5513865422798727</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1428,7 +1973,7 @@
         <v>1.6102896222109551</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1469,7 +2014,7 @@
         <v>1.5721439933535626</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1510,7 +2055,7 @@
         <v>1.4575904591220445</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -1551,7 +2096,7 @@
         <v>0.87970925770379738</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -1592,7 +2137,7 @@
         <v>1.5906200896864</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -1633,7 +2178,7 @@
         <v>0.94852003808943053</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -1674,7 +2219,7 @@
         <v>0.86748208809787286</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -1715,7 +2260,7 @@
         <v>0.69895389543999042</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -1756,7 +2301,7 @@
         <v>0.4926449324614085</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A29" s="5" t="s">
         <v>41</v>
       </c>
@@ -1797,7 +2342,7 @@
         <v>0.42147672834822086</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -1838,7 +2383,7 @@
         <v>1.7835210453348103</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -1879,7 +2424,7 @@
         <v>0.99999300667023794</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -1920,7 +2465,7 @@
         <v>0.92537957776179491</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A33" s="5" t="s">
         <v>45</v>
       </c>
@@ -1961,7 +2506,7 @@
         <v>0.90464464801410727</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A34" s="5" t="s">
         <v>46</v>
       </c>
@@ -2002,7 +2547,7 @@
         <v>0.45046073498041417</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -2043,11 +2588,11 @@
         <v>1.9171399723348523</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A38" s="7" t="s">
         <v>59</v>
       </c>
@@ -2084,7 +2629,7 @@
         <v>7.5586067541422424E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A39" s="7" t="s">
         <v>60</v>
       </c>
@@ -2121,119 +2666,119 @@
         <v>3.9410381849014544E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.5">
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.5">
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.5">
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.5">
       <c r="G56" s="2"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A57" s="4"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.5">
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.5">
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.5">
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.5">
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.5">
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.5">
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.5">
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D77" s="2"/>
     </row>
   </sheetData>
@@ -2249,23 +2794,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="18.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="31.5" style="1" customWidth="1"/>
-    <col min="2" max="14" width="18.83203125" style="1"/>
-    <col min="15" max="15" width="18.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="18.83203125" style="1"/>
+    <col min="2" max="14" width="18.8125" style="1"/>
+    <col min="15" max="15" width="18.8125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="18.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2309,7 +2854,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -2328,7 +2873,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2375,7 +2920,7 @@
         <v>1331954984895.5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2422,7 +2967,7 @@
         <v>6592402252</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2469,7 +3014,7 @@
         <v>23981048</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2516,12 +3061,12 @@
         <v>8210045</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -2568,7 +3113,7 @@
         <v>266390996.97909999</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -2615,7 +3160,7 @@
         <v>1318480.4504</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -2662,7 +3207,7 @@
         <v>4796.2096000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2714,15 +3259,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update clang and nodejs with nosmt results
</commit_message>
<xml_diff>
--- a/clang.xlsx
+++ b/clang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xdong\OneDrive\Paper\git_hub\shared_ptp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_F740F62D79B1ADD581DB163033E2D3777A84950E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{57070D98-D299-42DE-90C3-819FED3CFB21}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_F740F62D79B1ADD581DB163033E2D3777A84950E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{476876CB-7737-4087-8220-1227893C5F20}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
   <si>
     <t>CPU_CLK_UNHALTED.THREAD_P</t>
   </si>
@@ -289,6 +289,15 @@
   </si>
   <si>
     <t>4 hyperthreads/2cores</t>
+  </si>
+  <si>
+    <t>SMT</t>
+  </si>
+  <si>
+    <t>no STMT</t>
+  </si>
+  <si>
+    <t>2 processes/2 cores</t>
   </si>
 </sst>
 </file>
@@ -299,7 +308,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -364,6 +373,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -394,7 +411,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -406,15 +423,16 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -704,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B384F6F9-A13C-42B9-8587-294C53F132BC}">
-  <dimension ref="A2:I19"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -717,6 +735,11 @@
     <col min="7" max="9" width="9.0625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>82</v>
@@ -727,423 +750,614 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="78.75" x14ac:dyDescent="0.5">
-      <c r="A6" s="11"/>
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A6" s="10"/>
+      <c r="B6" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>269559340.06045002</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>270584219.91035002</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>254979371.49505001</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>254972036.48005</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10">
         <f>C7/B7</f>
         <v>1.0038020565329704</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <f>D7/B7</f>
         <v>0.94591184055380761</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <f>E7/B7</f>
         <v>0.94588462942100715</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>47708.169950000003</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>47066.353499999997</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <v>3474.0246000000002</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>2698.9146500000002</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10">
         <f t="shared" ref="G8:G19" si="0">C8/B8</f>
         <v>0.98654703270587296</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <f t="shared" ref="H8:H19" si="1">D8/B8</f>
         <v>7.2818232257512952E-2</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <f t="shared" ref="I8:I19" si="2">E8/B8</f>
         <v>5.6571330504367835E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>2674726.7326000002</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>2690581.50055</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>193823.9283</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>148097.10935000001</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <f t="shared" si="0"/>
         <v>1.0059276215984083</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <f t="shared" si="1"/>
         <v>7.2464946021454354E-2</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <f t="shared" si="2"/>
         <v>5.5369061648417608E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>14931593.6647</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>15033360.7807</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>5605997.9632999999</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>5554597.0680999998</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10">
         <f t="shared" si="0"/>
         <v>1.0068155562149128</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <f t="shared" si="1"/>
         <v>0.37544538708907021</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <f t="shared" si="2"/>
         <v>0.37200296182929921</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>269532641.56809998</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>270569085.08074999</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>254972162.96145001</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>254927708.68669999</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
         <f t="shared" si="0"/>
         <v>1.0038453357879777</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <f t="shared" si="1"/>
         <v>0.94597879306217125</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <f t="shared" si="2"/>
         <v>0.94581386211172525</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>19342.494200000001</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>19324.010600000001</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>3853.5345499999999</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>3631.0277500000002</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10">
         <f t="shared" si="0"/>
         <v>0.99904440452152243</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <f t="shared" si="1"/>
         <v>0.19922635158396479</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <f t="shared" si="2"/>
         <v>0.18772282997505046</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>1585133.47765</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>1620427.36555</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>656908.25349999999</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>646197.75254999998</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10">
         <f t="shared" si="0"/>
         <v>1.022265562110469</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <f t="shared" si="1"/>
         <v>0.41441825736586102</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <f t="shared" si="2"/>
         <v>0.40766141253164639</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>10896.971149999999</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>10753.867550000001</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <v>9352.0624499999994</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>8825.4004999999997</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10">
         <f t="shared" si="0"/>
         <v>0.98686758017157838</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="10">
         <f t="shared" si="1"/>
         <v>0.85822586122933797</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="10">
         <f t="shared" si="2"/>
         <v>0.80989482109439193</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>538604.22155000002</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>550671.14994999999</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <v>437690.78615</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>420984.0122</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10">
         <f t="shared" si="0"/>
         <v>1.0224040731899087</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <f t="shared" si="1"/>
         <v>0.81263898171909899</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="10">
         <f t="shared" si="2"/>
         <v>0.78162033522219421</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>47723.016049999998</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>47050.125950000001</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>3466.6095500000001</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>2695.7633000000001</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10">
         <f t="shared" si="0"/>
         <v>0.98590009274990076</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <f t="shared" si="1"/>
         <v>7.2640202504552318E-2</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <f t="shared" si="2"/>
         <v>5.6487697616923779E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>2676890.3783499999</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>2692992.3051</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <v>193731.09755000001</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>148404.8449</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10">
         <f t="shared" si="0"/>
         <v>1.0060151610541201</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="10">
         <f t="shared" si="1"/>
         <v>7.2371696322287696E-2</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="10">
         <f t="shared" si="2"/>
         <v>5.5439268675422856E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>14933141.28015</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>15035233.9946</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <v>5608488.4069499997</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>5552873.8894499997</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11">
+      <c r="F18" s="10"/>
+      <c r="G18" s="10">
         <f t="shared" si="0"/>
         <v>1.006836653623957</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <f t="shared" si="1"/>
         <v>0.37557325024475119</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="10">
         <f t="shared" si="2"/>
         <v>0.3718490159087427</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="10">
         <v>434.24299999999999</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <v>435.87299999999999</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="10">
         <v>400.45499999999998</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>400.55799999999999</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11">
+      <c r="F19" s="10"/>
+      <c r="G19" s="10">
         <f t="shared" si="0"/>
         <v>1.00375365866577</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="10">
         <f t="shared" si="1"/>
         <v>0.92219103128893265</v>
       </c>
-      <c r="I19" s="11">
-        <f t="shared" si="2"/>
+      <c r="I19" s="10">
+        <f t="shared" si="2"/>
+        <v>0.92242822567088012</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A25" s="10"/>
+      <c r="B25" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A26" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="10">
+        <v>184420794.1561</v>
+      </c>
+      <c r="C26" s="10">
+        <v>184868386.28560001</v>
+      </c>
+      <c r="D26" s="10">
+        <v>176087715.4878</v>
+      </c>
+      <c r="E26" s="10">
+        <v>176048390.85710001</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10">
+        <f>C26/B26</f>
+        <v>1.0024270155193082</v>
+      </c>
+      <c r="H26" s="10">
+        <f>D26/B26</f>
+        <v>0.95481486398303539</v>
+      </c>
+      <c r="I26" s="10">
+        <f>E26/B26</f>
+        <v>0.95460163081223204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A27" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="10">
+        <v>1208581.8125</v>
+      </c>
+      <c r="C27" s="10">
+        <v>1224992.8533000001</v>
+      </c>
+      <c r="D27" s="10">
+        <v>749348.17200000002</v>
+      </c>
+      <c r="E27" s="10">
+        <v>742821.42469999997</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10">
+        <f t="shared" ref="G27:G30" si="3">C27/B27</f>
+        <v>1.0135787586990517</v>
+      </c>
+      <c r="H27" s="10">
+        <f t="shared" ref="H27:H30" si="4">D27/B27</f>
+        <v>0.62002271112283514</v>
+      </c>
+      <c r="I27" s="10">
+        <f t="shared" ref="I27:I30" si="5">E27/B27</f>
+        <v>0.61462237559528055</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A28" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="10">
+        <v>461685.00760000001</v>
+      </c>
+      <c r="C28" s="10">
+        <v>462376.4534</v>
+      </c>
+      <c r="D28" s="10">
+        <v>422278.59110000002</v>
+      </c>
+      <c r="E28" s="10">
+        <v>396182.16840000002</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0014976570358962</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="4"/>
+        <v>0.91464653204822843</v>
+      </c>
+      <c r="I28" s="10">
+        <f t="shared" si="5"/>
+        <v>0.85812223026147927</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A29" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="10">
+        <v>1709616.3977999999</v>
+      </c>
+      <c r="C29" s="10">
+        <v>1694467.3581999999</v>
+      </c>
+      <c r="D29" s="10">
+        <v>210361.14249999999</v>
+      </c>
+      <c r="E29" s="10">
+        <v>161322.48240000001</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10">
+        <f t="shared" si="3"/>
+        <v>0.99113892472048448</v>
+      </c>
+      <c r="H29" s="10">
+        <f t="shared" si="4"/>
+        <v>0.12304581470480792</v>
+      </c>
+      <c r="I29" s="10">
+        <f t="shared" si="5"/>
+        <v>9.4361801049402644E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A30" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="10">
+        <v>434.24299999999999</v>
+      </c>
+      <c r="C30" s="10">
+        <v>435.87299999999999</v>
+      </c>
+      <c r="D30" s="10">
+        <v>400.45499999999998</v>
+      </c>
+      <c r="E30" s="10">
+        <v>400.55799999999999</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10">
+        <f t="shared" si="3"/>
+        <v>1.00375365866577</v>
+      </c>
+      <c r="H30" s="10">
+        <f t="shared" si="4"/>
+        <v>0.92219103128893265</v>
+      </c>
+      <c r="I30" s="10">
+        <f t="shared" si="5"/>
         <v>0.92242822567088012</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1176,41 +1390,41 @@
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" s="4"/>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="9"/>
+      <c r="J2" s="13"/>
       <c r="K2" s="6" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Latest results and figures
</commit_message>
<xml_diff>
--- a/clang.xlsx
+++ b/clang.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xdong\OneDrive\Paper\git_hub\shared_ptp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_F740F62D79B1ADD581DB163033E2D3777A84950E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{A3E0E4DB-451F-40D3-B556-ECA0D800FA5C}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="11_F740F62D79B1ADD581DB163033E2D3777A84950E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B2FC4EFF-F826-4C6B-B3C7-B63915C76F5C}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
   <si>
     <t>CPU_CLK_UNHALTED.THREAD_P</t>
   </si>
@@ -252,33 +252,12 @@
     <t>Col E/ Col B</t>
   </si>
   <si>
-    <t>DTLB_LOAD_MISSES.WALK_COMPLETED</t>
-  </si>
-  <si>
-    <t>DTLB_LOAD_MISSES.WALK_PENDING</t>
-  </si>
-  <si>
-    <t>DTLB_STORE_MISSES.WALK_COMPLETED</t>
-  </si>
-  <si>
-    <t>DTLB_STORE_MISSES.WALK_PENDING</t>
-  </si>
-  <si>
-    <t>ITLB_MISSES.WALK_PENDING</t>
-  </si>
-  <si>
-    <t>ICACHE_64B.IFTAG_STALL</t>
-  </si>
-  <si>
     <t>CPU_CLK_UNHALTED.THREAD_P (os + usr)</t>
   </si>
   <si>
     <t>INST_RETIRED.ANY_P</t>
   </si>
   <si>
-    <t>elapse time</t>
-  </si>
-  <si>
     <t>SMT</t>
   </si>
   <si>
@@ -310,6 +289,9 @@
   </si>
   <si>
     <t>averaged over 5000 iterations x 2cores</t>
+  </si>
+  <si>
+    <t>INST_RETIRED.ANY_P (os + usr)</t>
   </si>
 </sst>
 </file>
@@ -423,7 +405,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -445,7 +427,6 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -738,7 +719,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -750,12 +731,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
@@ -784,304 +765,285 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A7" s="11" t="s">
-        <v>0</v>
+      <c r="A7" t="s">
+        <v>75</v>
       </c>
       <c r="B7" s="10">
-        <v>269559340.06045002</v>
+        <v>269553674.51539999</v>
       </c>
       <c r="C7" s="10">
-        <v>270584219.91035002</v>
+        <v>270613181.92799997</v>
       </c>
       <c r="D7" s="10">
-        <v>254979371.49505001</v>
+        <v>254968323.70770001</v>
       </c>
       <c r="E7" s="10">
-        <v>254972036.48005</v>
+        <v>254986394.25944999</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10">
         <f>C7/B7</f>
-        <v>1.0038020565329704</v>
+        <v>1.0039305990337721</v>
       </c>
       <c r="H7" s="10">
         <f>D7/B7</f>
-        <v>0.94591184055380761</v>
+        <v>0.94589073647791544</v>
       </c>
       <c r="I7" s="10">
         <f>E7/B7</f>
-        <v>0.94588462942100715</v>
+        <v>0.94595777526632174</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A8" s="11" t="s">
-        <v>1</v>
+      <c r="A8" t="s">
+        <v>76</v>
       </c>
       <c r="B8" s="10">
-        <v>47708.169950000003</v>
+        <v>1587749.1723499999</v>
       </c>
       <c r="C8" s="10">
-        <v>47066.353499999997</v>
+        <v>1623758.652</v>
       </c>
       <c r="D8" s="10">
-        <v>3474.0246000000002</v>
+        <v>657411.55735000002</v>
       </c>
       <c r="E8" s="10">
-        <v>2698.9146500000002</v>
+        <v>647626.05870000005</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10">
-        <f t="shared" ref="G8:G19" si="0">C8/B8</f>
-        <v>0.98654703270587296</v>
+        <f t="shared" ref="G8:G15" si="0">C8/B8</f>
+        <v>1.0226795770245642</v>
       </c>
       <c r="H8" s="10">
-        <f t="shared" ref="H8:H19" si="1">D8/B8</f>
-        <v>7.2818232257512952E-2</v>
+        <f t="shared" ref="H8:H15" si="1">D8/B8</f>
+        <v>0.41405252718663149</v>
       </c>
       <c r="I8" s="10">
-        <f t="shared" ref="I8:I19" si="2">E8/B8</f>
-        <v>5.6571330504367835E-2</v>
+        <f t="shared" ref="I8:I15" si="2">E8/B8</f>
+        <v>0.40788940090673137</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A9" s="11" t="s">
-        <v>75</v>
+      <c r="A9" t="s">
+        <v>77</v>
       </c>
       <c r="B9" s="10">
-        <v>2674726.7326000002</v>
+        <v>539639.92255000002</v>
       </c>
       <c r="C9" s="10">
-        <v>2690581.50055</v>
+        <v>549522.79244999995</v>
       </c>
       <c r="D9" s="10">
-        <v>193823.9283</v>
+        <v>435870.00605000003</v>
       </c>
       <c r="E9" s="10">
-        <v>148097.10935000001</v>
+        <v>418838.23664999998</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10">
         <f t="shared" si="0"/>
-        <v>1.0059276215984083</v>
+        <v>1.0183138227677813</v>
       </c>
       <c r="H9" s="10">
         <f t="shared" si="1"/>
-        <v>7.2464946021454354E-2</v>
+        <v>0.8077052638921739</v>
       </c>
       <c r="I9" s="10">
         <f t="shared" si="2"/>
-        <v>5.5369061648417608E-2</v>
+        <v>0.77614390475566186</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A10" s="11" t="s">
-        <v>76</v>
+      <c r="A10" t="s">
+        <v>78</v>
       </c>
       <c r="B10" s="10">
-        <v>14931593.6647</v>
+        <v>2683057.7054499998</v>
       </c>
       <c r="C10" s="10">
-        <v>15033360.7807</v>
+        <v>2691092.7038500002</v>
       </c>
       <c r="D10" s="10">
-        <v>5605997.9632999999</v>
+        <v>193876.04384999999</v>
       </c>
       <c r="E10" s="10">
-        <v>5554597.0680999998</v>
+        <v>148342.50774999999</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10">
         <f t="shared" si="0"/>
-        <v>1.0068155562149128</v>
+        <v>1.0029947169543463</v>
       </c>
       <c r="H10" s="10">
         <f t="shared" si="1"/>
-        <v>0.37544538708907021</v>
+        <v>7.2259364178484303E-2</v>
       </c>
       <c r="I10" s="10">
         <f t="shared" si="2"/>
-        <v>0.37200296182929921</v>
+        <v>5.5288601303161364E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A11" s="11" t="s">
-        <v>77</v>
+      <c r="A11" t="s">
+        <v>79</v>
       </c>
       <c r="B11" s="10">
-        <v>269532641.56809998</v>
+        <v>14934563.44795</v>
       </c>
       <c r="C11" s="10">
-        <v>270569085.08074999</v>
+        <v>15033884.34285</v>
       </c>
       <c r="D11" s="10">
-        <v>254972162.96145001</v>
+        <v>5605968.9563999996</v>
       </c>
       <c r="E11" s="10">
-        <v>254927708.68669999</v>
+        <v>5555615.6648000004</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10">
         <f t="shared" si="0"/>
-        <v>1.0038453357879777</v>
+        <v>1.0066504049647085</v>
       </c>
       <c r="H11" s="10">
         <f t="shared" si="1"/>
-        <v>0.94597879306217125</v>
+        <v>0.37536878636847637</v>
       </c>
       <c r="I11" s="10">
         <f t="shared" si="2"/>
-        <v>0.94581386211172525</v>
+        <v>0.37199719189398833</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A12" s="15" t="s">
+      <c r="A12" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="10">
-        <v>19342.494200000001</v>
+        <v>298525048.25484997</v>
       </c>
       <c r="C12" s="10">
-        <v>19324.010600000001</v>
+        <v>299636984.59315002</v>
       </c>
       <c r="D12" s="10">
-        <v>3853.5345499999999</v>
+        <v>278691753.02929997</v>
       </c>
       <c r="E12" s="10">
-        <v>3631.0277500000002</v>
+        <v>278672485.94489998</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10">
         <f t="shared" si="0"/>
-        <v>0.99904440452152243</v>
+        <v>1.0037247673011036</v>
       </c>
       <c r="H12" s="10">
         <f t="shared" si="1"/>
-        <v>0.19922635158396479</v>
+        <v>0.93356237494477057</v>
       </c>
       <c r="I12" s="10">
         <f t="shared" si="2"/>
-        <v>0.18772282997505046</v>
+        <v>0.93349783401424358</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A13" s="15" t="s">
-        <v>72</v>
+      <c r="A13" t="s">
+        <v>84</v>
       </c>
       <c r="B13" s="10">
-        <v>1585133.47765</v>
+        <v>249681812.76295</v>
       </c>
       <c r="C13" s="10">
-        <v>1620427.36555</v>
+        <v>249649361.74445</v>
       </c>
       <c r="D13" s="10">
-        <v>656908.25349999999</v>
+        <v>239455846.833</v>
       </c>
       <c r="E13" s="10">
-        <v>646197.75254999998</v>
+        <v>239755297.35315001</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10">
         <f t="shared" si="0"/>
-        <v>1.022265562110469</v>
+        <v>0.99987003050746504</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="1"/>
-        <v>0.41441825736586102</v>
+        <v>0.95904400958647873</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="2"/>
-        <v>0.40766141253164639</v>
+        <v>0.96024333811119711</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A14" s="15" t="s">
-        <v>73</v>
+      <c r="A14" t="s">
+        <v>80</v>
       </c>
       <c r="B14" s="10">
-        <v>10896.971149999999</v>
+        <v>223635326.6234</v>
       </c>
       <c r="C14" s="10">
-        <v>10753.867550000001</v>
+        <v>223635313.88734999</v>
       </c>
       <c r="D14" s="10">
-        <v>9352.0624499999994</v>
+        <v>223635302.04449999</v>
       </c>
       <c r="E14" s="10">
-        <v>8825.4004999999997</v>
+        <v>223635180.03619999</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10">
         <f t="shared" si="0"/>
-        <v>0.98686758017157838</v>
+        <v>0.99999994304991879</v>
       </c>
       <c r="H14" s="10">
         <f t="shared" si="1"/>
-        <v>0.85822586122933797</v>
+        <v>0.99999989009383994</v>
       </c>
       <c r="I14" s="10">
         <f t="shared" si="2"/>
-        <v>0.80989482109439193</v>
+        <v>0.99999934452574091</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A15" s="15" t="s">
-        <v>74</v>
+      <c r="A15" t="s">
+        <v>81</v>
       </c>
       <c r="B15" s="10">
-        <v>538604.22155000002</v>
+        <v>434.46350000000001</v>
       </c>
       <c r="C15" s="10">
-        <v>550671.14994999999</v>
+        <v>436.22449999999998</v>
       </c>
       <c r="D15" s="10">
-        <v>437690.78615</v>
+        <v>400.39800000000002</v>
       </c>
       <c r="E15" s="10">
-        <v>420984.0122</v>
+        <v>400.3895</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10">
         <f t="shared" si="0"/>
-        <v>1.0224040731899087</v>
+        <v>1.0040532749011135</v>
       </c>
       <c r="H15" s="10">
         <f t="shared" si="1"/>
-        <v>0.81263898171909899</v>
+        <v>0.92159180230330051</v>
       </c>
       <c r="I15" s="10">
         <f t="shared" si="2"/>
-        <v>0.78162033522219421</v>
+        <v>0.92157223794403897</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A16" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="10">
-        <v>434.24299999999999</v>
-      </c>
-      <c r="C16" s="10">
-        <v>435.87299999999999</v>
-      </c>
-      <c r="D16" s="10">
-        <v>400.45499999999998</v>
-      </c>
-      <c r="E16" s="10">
-        <v>400.55799999999999</v>
-      </c>
+      <c r="A16" s="12"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="10">
-        <f>C16/B16</f>
-        <v>1.00375365866577</v>
-      </c>
-      <c r="H16" s="10">
-        <f>D16/B16</f>
-        <v>0.92219103128893265</v>
-      </c>
-      <c r="I16" s="10">
-        <f>E16/B16</f>
-        <v>0.92242822567088012</v>
-      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" s="11"/>
@@ -1107,12 +1069,12 @@
     </row>
     <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
@@ -1142,7 +1104,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B26" s="10">
         <v>184426445.3026</v>
@@ -1172,7 +1134,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B27" s="10">
         <v>1207408.2644</v>
@@ -1202,7 +1164,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B28" s="10">
         <v>462922.9351</v>
@@ -1232,7 +1194,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B29" s="10">
         <v>1708458.0157000001</v>
@@ -1262,7 +1224,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B30" s="10">
         <v>7757916.3880000003</v>
@@ -1292,7 +1254,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B31" s="10">
         <v>203852047.95969999</v>
@@ -1321,7 +1283,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B32" s="10">
         <v>250759229.21380001</v>
@@ -1350,7 +1312,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B33" s="10">
         <v>223753374.2789</v>
@@ -1379,7 +1341,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B34" s="10">
         <v>294.29500000000002</v>

</xml_diff>